<commit_message>
More extensive testing of search
</commit_message>
<xml_diff>
--- a/oppgave_3/cypress/downloads/Lunsjliste.xlsx
+++ b/oppgave_3/cypress/downloads/Lunsjliste.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="18">
   <si>
     <t>Uke</t>
   </si>
@@ -25,37 +25,43 @@
     <t>Lunsj</t>
   </si>
   <si>
+    <t>Mandag</t>
+  </si>
+  <si>
+    <t>Susanne</t>
+  </si>
+  <si>
+    <t>Sushi</t>
+  </si>
+  <si>
+    <t>Onsdag</t>
+  </si>
+  <si>
+    <t>Fredag</t>
+  </si>
+  <si>
+    <t>Poteter og fisk</t>
+  </si>
+  <si>
+    <t>Lasagne</t>
+  </si>
+  <si>
     <t>Torsdag</t>
   </si>
   <si>
-    <t>Trine</t>
-  </si>
-  <si>
-    <t>Lammeribbe</t>
-  </si>
-  <si>
-    <t>Mandag</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Fredag</t>
-  </si>
-  <si>
-    <t>Spaghetti og kjøttsaus</t>
-  </si>
-  <si>
-    <t>Egg og bacon</t>
-  </si>
-  <si>
-    <t>Poteter og fisk</t>
-  </si>
-  <si>
     <t>Brødskiver med pålegg</t>
   </si>
   <si>
     <t>Tirsdag</t>
+  </si>
+  <si>
+    <t>Salat</t>
+  </si>
+  <si>
+    <t>Pasta bolognese</t>
+  </si>
+  <si>
+    <t>Ris og kylling</t>
   </si>
   <si>
     <t>Pølser</t>
@@ -435,7 +441,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="4" width="10" customWidth="1"/>
@@ -457,7 +463,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -471,7 +477,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -480,43 +486,43 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -527,72 +533,114 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
         <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
       </c>
       <c r="D11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>39</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>49</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>